<commit_message>
upd output, create temp_file and unique_temp_file, logic for replace, need replace data dict
</commit_message>
<xml_diff>
--- a/audac_parse_test/prod/results/audac_parser_result.xlsx
+++ b/audac_parse_test/prod/results/audac_parser_result.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Характеристика</t>
+          <t>Тип АС</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -436,7 +436,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Значение</t>
+          <t>Широкополосная</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Speaker type</t>
+          <t>Пиковая мощность</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -458,7 +458,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Full range</t>
+          <t>140 W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -470,7 +470,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Peak power handling</t>
+          <t>Program power handling</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>140 W</t>
+          <t>70 W</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Program power handling</t>
+          <t>Продолжительная мощность</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>70 W</t>
+          <t>35 W</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -514,7 +514,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RMS/AES power handling</t>
+          <t>Impedance</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>35 W</t>
+          <t>8 Ω (ATEO4)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -536,7 +536,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Impedance</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8 Ω (ATEO4)</t>
+          <t>16 Ω (ATEO4D)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -558,17 +558,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Incline angle</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>-</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>16 Ω (ATEO4D)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Incline angle</t>
+          <t xml:space="preserve">          Left</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>30°</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -602,7 +602,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Left</t>
+          <t xml:space="preserve">          Right</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Right</t>
+          <t xml:space="preserve">          Bottom</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -646,7 +646,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Bottom</t>
+          <t xml:space="preserve">          Top</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>30°</t>
+          <t>5°</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Top</t>
+          <t>Sensitivity (1W/1m)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5°</t>
+          <t>86 dB</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -690,7 +690,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sensitivity (1W/1m)</t>
+          <t>Sound Pressure (Max. W/1m)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>86 dB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sound Pressure (Max. W/1m)</t>
+          <t xml:space="preserve">          @ 8 Ω</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>101 dB</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -734,7 +734,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">          @ 8 Ω</t>
+          <t xml:space="preserve">          @ 100 V</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>101 dB</t>
+          <t>100 dB</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">          @ 100 V</t>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>100 dB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -778,7 +778,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t xml:space="preserve">          Отклик (± 3 дБ)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -788,7 +788,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>100 Hz - 20 kHz</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -800,7 +800,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Response (± 3 dB)</t>
+          <t xml:space="preserve">          Range (-10 dB)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>100 Hz - 20 kHz</t>
+          <t>65 Hz - 20 kHz</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -822,7 +822,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Range (-10 dB)</t>
+          <t>Dispersion</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>65 Hz - 20 kHz</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dispersion</t>
+          <t xml:space="preserve">          Horizontal</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>130°</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -866,7 +866,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Horizontal</t>
+          <t xml:space="preserve">          Vertical</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Vertical</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -898,7 +898,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>130°</t>
+          <t>6-pin Custom Terminal Block</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -910,7 +910,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Drivers</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6-pin Custom Terminal Block</t>
+          <t>1” Dome tweeter</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -932,7 +932,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Drivers</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1” Dome tweeter</t>
+          <t>4” MF / LF Woofer</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -954,17 +954,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Line Transformer Tappings</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>-</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>4” MF / LF Woofer</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Line Transformer Tappings</t>
+          <t xml:space="preserve">          1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>208 Ω - 100 В / Нет - 70 В / 24 Вт</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">          1</t>
+          <t xml:space="preserve">          2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>208 Ω - 100 V / Not used - 70 V / 24 W</t>
+          <t>417 Ω - 100 V / 24 W - 70 V / 12 W</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1020,7 +1020,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">          2</t>
+          <t xml:space="preserve">          3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>417 Ω - 100 V / 24 W - 70 V / 12 W</t>
+          <t>833 Ω - 100 V / 12 W - 70 V / 6 W</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1042,7 +1042,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve">          3</t>
+          <t xml:space="preserve">          4</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>833 Ω - 100 V / 12 W - 70 V / 6 W</t>
+          <t>1667 Ω - 100 V / 6 W - 70 V / 3 W</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1064,7 +1064,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">          4</t>
+          <t>Dimensions</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1667 Ω - 100 V / 6 W - 70 V / 3 W</t>
+          <t>136 x 244 x 153 mm (W x H x D)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1086,7 +1086,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dimensions</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>136 x 244 x 153 mm (W x H x D)</t>
+          <t>2.050 kg</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>Operating temperature</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.050 kg</t>
+          <t>-20 °C ~ 60 °C</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1130,7 +1130,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Operating temperature</t>
+          <t>Mounting</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>-20 °C ~ 60 °C</t>
+          <t>Clevermount™</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1152,7 +1152,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mounting</t>
+          <t>Accessories</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Clevermount™</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1174,7 +1174,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Accessories</t>
+          <t xml:space="preserve">          Included</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Allen-key wrench</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1196,7 +1196,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Included</t>
+          <t>Construction</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Allen-key wrench</t>
+          <t>ABS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1218,7 +1218,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Construction</t>
+          <t>Front finish</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ABS</t>
+          <t>Steel grill</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Front finish</t>
+          <t>Colours</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Steel grill</t>
+          <t>Black (RAL9005) (ATEO4/B, ATEO4D/B)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1262,7 +1262,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Colours</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1272,32 +1272,10 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Black (RAL9005) (ATEO4/B, ATEO4D/B)</t>
+          <t>White (RAL9003) (ATEO4/W, ATEO4D/W)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
-        <is>
-          <t>||</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>White (RAL9003) (ATEO4/W, ATEO4D/W)</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
         <is>
           <t>||</t>
         </is>
@@ -1314,7 +1292,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1325,7 +1303,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Характеристика</t>
+          <t>Тип АС</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1335,7 +1313,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Значение</t>
+          <t>2-way coaxial</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -1347,7 +1325,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Speaker type</t>
+          <t>Пиковая мощность</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1357,7 +1335,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2-way coaxial</t>
+          <t>240 W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1369,7 +1347,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Peak power handling</t>
+          <t>Program power handling</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1379,7 +1357,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>240 W</t>
+          <t>120 W</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1391,7 +1369,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Program power handling</t>
+          <t>Продолжительная мощность</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1401,7 +1379,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>120 W</t>
+          <t>60 W</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1413,7 +1391,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RMS/AES power handling</t>
+          <t>Impedance</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1423,7 +1401,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>60 W</t>
+          <t>16 Ω</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1435,7 +1413,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Impedance</t>
+          <t>Line Transformer Tappings</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1445,7 +1423,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16 Ω</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1457,7 +1435,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Line Transformer Tappings</t>
+          <t xml:space="preserve">          1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1467,7 +1445,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>83 Ω - 100 V / Not used - 70 V / 60 W</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1479,7 +1457,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">          1</t>
+          <t xml:space="preserve">          2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1489,7 +1467,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>83 Ω - 100 V / Not used - 70 V / 60 W</t>
+          <t>167 Ω - 100 V / 60 W - 70 V / 30 W</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1501,7 +1479,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">          2</t>
+          <t xml:space="preserve">          3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1511,7 +1489,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>167 Ω - 100 V / 60 W - 70 V / 30 W</t>
+          <t>333 Ω - 100 V / 30 W - 70 V / 15 W</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1523,7 +1501,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">          3</t>
+          <t xml:space="preserve">          4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1533,7 +1511,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>333 Ω - 100 V / 30 W - 70 V / 15 W</t>
+          <t>667 Ω - 100 V / 15 W - 70 V / 7.5 W</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1545,7 +1523,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">          4</t>
+          <t>Dispersion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1555,7 +1533,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>667 Ω - 100 V / 15 W - 70 V / 7.5 W</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1567,7 +1545,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dispersion</t>
+          <t xml:space="preserve">          Conical</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1577,7 +1555,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>115° (average 500 Hz to 5 kHz @ -6 dB)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1589,7 +1567,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Conical</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1599,7 +1577,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>115° (average 500 Hz to 5 kHz @ -6 dB)</t>
+          <t>4-pin Euro Terminal Block</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1611,7 +1589,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Sensitivity (1W/1m)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1621,7 +1599,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4-pin Euro Terminal Block</t>
+          <t>83 dB</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1633,7 +1611,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sensitivity (1W/1m)</t>
+          <t>Sound Pressure (Max. W/1m)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1643,7 +1621,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>83 dB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1655,7 +1633,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sound Pressure (Max. W/1m)</t>
+          <t xml:space="preserve">          @ 16 Ω</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1665,7 +1643,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>101 dB</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1677,7 +1655,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">          @ 16 Ω</t>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1687,7 +1665,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>101 dB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1699,7 +1677,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t xml:space="preserve">          Range (-10 dB)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1709,7 +1687,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>61.5 Hz - 20 kHz</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1721,7 +1699,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Range (-10 dB)</t>
+          <t xml:space="preserve">          Отклик (± 3 дБ)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1731,7 +1709,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>61.5 Hz - 20 kHz</t>
+          <t>75 Hz - 17 kHz</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1743,7 +1721,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Response (± 3 dB)</t>
+          <t>Dimensions</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1753,7 +1731,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>75 Hz - 17 kHz</t>
+          <t>230 x 302 mm (Ø x H)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1765,7 +1743,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dimensions</t>
+          <t>Connection cable length</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1775,7 +1753,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>230 x 302 mm (Ø x H)</t>
+          <t>3.5 m</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1787,7 +1765,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Connection cable length</t>
+          <t>Construction</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1797,7 +1775,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>3.5 m</t>
+          <t>Polypropylene</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1809,7 +1787,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Construction</t>
+          <t>Front finish</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1819,7 +1797,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Polypropylene</t>
+          <t>Aluminium grill</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1831,7 +1809,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Front finish</t>
+          <t>Mounting &amp; handling</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1841,7 +1819,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Aluminium grill</t>
+          <t>Dual snap hook and dual Gripple™ hanger</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1853,7 +1831,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mounting &amp; handling</t>
+          <t>Accessories</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1863,7 +1841,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Dual snap hook and dual Gripple™ hanger</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1875,7 +1853,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Accessories</t>
+          <t xml:space="preserve">          Included</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1885,7 +1863,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Connection cable with dual steel core, snap hook &amp; open ends – 3.5 meter</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1897,7 +1875,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Included</t>
+          <t xml:space="preserve">          -</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1907,7 +1885,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Connection cable with dual steel core, snap hook &amp; open ends – 3.5 meter</t>
+          <t>2 Gripple™ hangers</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1919,7 +1897,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">          -</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1929,32 +1907,10 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2 Gripple™ hangers</t>
+          <t>3.39 kg</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
-        <is>
-          <t>||</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Weight</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>3.39 kg</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
         <is>
           <t>||</t>
         </is>
@@ -1971,7 +1927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1982,7 +1938,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Характеристика</t>
+          <t>Тип АС</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1992,7 +1948,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Значение</t>
+          <t>2-way</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -2004,7 +1960,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Speaker type</t>
+          <t>Пиковая мощность</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2014,7 +1970,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2-way</t>
+          <t>320 W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2026,7 +1982,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Peak power handling</t>
+          <t>Program power handling</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2036,7 +1992,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>320 W</t>
+          <t>160 W</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2048,7 +2004,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Program power handling</t>
+          <t>Продолжительная мощность</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2058,7 +2014,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>160 W</t>
+          <t>80 W</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2070,7 +2026,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RMS/AES power handling</t>
+          <t>Impedance</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2080,7 +2036,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>80 W</t>
+          <t>8 Ω</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2092,7 +2048,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Impedance</t>
+          <t>Sensitivity (1W/1m)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2102,7 +2058,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8 Ω</t>
+          <t>88 dB</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2114,7 +2070,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sensitivity (1W/1m)</t>
+          <t>Sound Pressure (Max. W/1m)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2124,7 +2080,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>88 dB</t>
+          <t>110 dB</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2136,7 +2092,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sound Pressure (Max. W/1m)</t>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2146,7 +2102,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>110 dB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2158,7 +2114,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t xml:space="preserve">          Отклик (± 3 дБ)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2168,7 +2124,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65 Hz - 18 kHz</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2180,7 +2136,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Response (± 3 dB)</t>
+          <t xml:space="preserve">          Range (-10 dB)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2190,7 +2146,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>65 Hz - 18 kHz</t>
+          <t>55 Hz - 20 kHz</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2202,7 +2158,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Range (-10 dB)</t>
+          <t>Crossover</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2212,7 +2168,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>55 Hz - 20 kHz</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2224,7 +2180,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Crossover</t>
+          <t xml:space="preserve">          Frequency</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2234,7 +2190,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.5 kHz</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2246,7 +2202,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Frequency</t>
+          <t xml:space="preserve">          Type</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2256,7 +2212,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.5 kHz</t>
+          <t>Passive built-in</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2268,7 +2224,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Type</t>
+          <t>Dispersion</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2278,7 +2234,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Passive built-in</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2290,7 +2246,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dispersion</t>
+          <t xml:space="preserve">          Horizontal</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2300,7 +2256,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>120°</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2312,7 +2268,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Horizontal</t>
+          <t xml:space="preserve">          Vertical</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2334,7 +2290,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Vertical</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2344,7 +2300,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>120°</t>
+          <t>4-pin Euro Terminal Block (Pitch - 5.08 mm)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2356,7 +2312,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Drivers</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2366,7 +2322,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4-pin Euro Terminal Block (Pitch - 5.08 mm)</t>
+          <t>1” Dome tweeter</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2378,7 +2334,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Drivers</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2388,7 +2344,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1” Dome tweeter</t>
+          <t>6” MF / LF Woofer</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2400,7 +2356,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dimensions</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2410,7 +2366,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6” MF / LF Woofer</t>
+          <t>210 x 345 x 220 mm (W x H x D)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2422,7 +2378,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dimensions</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2432,7 +2388,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>210 x 345 x 220 mm (W x H x D)</t>
+          <t>5.600 kg</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2444,7 +2400,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>Operating temperature</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2454,7 +2410,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5.600 kg</t>
+          <t>-20 °C ~ 60 °C</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2466,7 +2422,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Operating temperature</t>
+          <t>Construction</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2476,7 +2432,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>-20 °C ~ 60 °C</t>
+          <t>Medium Density Fibreboard with structured coating</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2488,7 +2444,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Construction</t>
+          <t>Front finish</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2498,7 +2454,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Medium Density Fibreboard with structured coating</t>
+          <t>Steel grill</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2510,7 +2466,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Front finish</t>
+          <t>Mounting &amp; handling</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2520,7 +2476,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Steel grill</t>
+          <t>2-way Revolving mounting bracket</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2532,7 +2488,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mounting &amp; handling</t>
+          <t>Colours</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2542,7 +2498,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2-way Revolving mounting bracket</t>
+          <t>Black (RAL9004) (XENO6/B)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2554,7 +2510,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Colours</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2564,7 +2520,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Black (RAL9004) (XENO6/B)</t>
+          <t>White (RAL9003) (XENO6/W)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2576,17 +2532,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>-</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>White (RAL9003) (XENO6/W)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2598,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Accessories</t>
+          <t xml:space="preserve">          Included</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2608,7 +2564,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>4-pin Euro Terminal Block (Pitch - 5.08 mm)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2620,7 +2576,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">          Included</t>
+          <t xml:space="preserve">          -</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2630,7 +2586,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4-pin Euro Terminal Block (Pitch - 5.08 mm)</t>
+          <t>2-way Revolving mounting bracket</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2642,7 +2598,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">          -</t>
+          <t xml:space="preserve">          Optional</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2652,32 +2608,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2-way Revolving mounting bracket</t>
+          <t>WBP100 Wall bracket mounting plate</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
-        <is>
-          <t>||</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">          Optional</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>WBP100 Wall bracket mounting plate</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
         <is>
           <t>||</t>
         </is>

</xml_diff>